<commit_message>
Added Cart Validation before processing order or shipment
</commit_message>
<xml_diff>
--- a/Warehouse/shipmentlog.xlsx
+++ b/Warehouse/shipmentlog.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="29400" windowHeight="12300"/>
+    <workbookView windowWidth="29400" windowHeight="12340"/>
   </bookViews>
   <sheets>
     <sheet name="Shipments" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" fullCalcOnLoad="1" fullPrecision="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -35,7 +35,7 @@
     <t>Hash</t>
   </si>
   <si>
-    <t>$2a$11$zAlZdsfwK54NR/S1tkHAAOyIx3PAQcVovBc643votsAysk/1jgIyO</t>
+    <t>$2a$11$WGwvur5fxBMFP3SjwgkXR.Qw/tu6.mLTWKC.CFXLXqPlTIjbUoNLa</t>
   </si>
 </sst>
 </file>
@@ -508,154 +508,154 @@
     </border>
   </borders>
   <cellStyleXfs count="49">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFill="0" applyBorder="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" applyFill="0" borderId="0" applyBorder="0"/>
+    <xf numFmtId="43" applyNumberFormat="1" fontId="1" applyFont="0" fillId="0" applyFill="0" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" applyNumberFormat="1" fontId="1" applyFont="0" fillId="0" applyFill="0" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" applyNumberFormat="1" fontId="1" applyFont="0" fillId="0" applyFill="0" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" applyNumberFormat="1" fontId="1" applyFont="0" fillId="0" applyFill="0" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" applyNumberFormat="1" fontId="1" applyFont="0" fillId="0" applyFill="0" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="2" applyFont="1" fillId="0" applyFill="0" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="3" applyFont="1" fillId="0" applyFill="0" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="1" applyFont="0" fillId="2" applyFill="1" borderId="1" applyBorder="1" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="4" applyFont="1" fillId="0" applyFill="0" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="5" applyFont="1" fillId="0" applyFill="0" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="6" applyFont="1" fillId="0" applyFill="0" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="7" applyFont="1" fillId="0" applyFill="0" borderId="2" applyBorder="1" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="8" applyFont="1" fillId="0" applyFill="0" borderId="2" applyBorder="1" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="9" applyFont="1" fillId="0" applyFill="0" borderId="3" applyBorder="1" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="9" applyFont="1" fillId="0" applyFill="0" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="10" applyFont="1" fillId="3" applyFill="1" borderId="4" applyBorder="1" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="11" applyFont="1" fillId="4" applyFill="1" borderId="5" applyBorder="1" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="12" applyFont="1" fillId="4" applyFill="1" borderId="4" applyBorder="1" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="13" applyFont="1" fillId="5" applyFill="1" borderId="6" applyBorder="1" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="14" applyFont="1" fillId="0" applyFill="0" borderId="7" applyBorder="1" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="15" applyFont="1" fillId="0" applyFill="0" borderId="8" applyBorder="1" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="16" applyFont="1" fillId="6" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="17" applyFont="1" fillId="7" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="18" applyFont="1" fillId="8" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="19" applyFont="1" fillId="9" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="20" applyFont="1" fillId="10" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="20" applyFont="1" fillId="11" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="19" applyFont="1" fillId="12" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="19" applyFont="1" fillId="13" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="20" applyFont="1" fillId="14" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="20" applyFont="1" fillId="15" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="19" applyFont="1" fillId="16" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="19" applyFont="1" fillId="17" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="20" applyFont="1" fillId="18" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="20" applyFont="1" fillId="19" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="19" applyFont="1" fillId="20" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="19" applyFont="1" fillId="21" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="20" applyFont="1" fillId="22" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="20" applyFont="1" fillId="23" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="19" applyFont="1" fillId="24" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="19" applyFont="1" fillId="25" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="20" applyFont="1" fillId="26" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="20" applyFont="1" fillId="27" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="19" applyFont="1" fillId="28" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="19" applyFont="1" fillId="29" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="20" applyFont="1" fillId="30" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="20" applyFont="1" fillId="31" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="19" applyFont="1" fillId="32" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" applyFill="0" borderId="0" applyBorder="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -905,18 +905,18 @@
       <tableStyleElement type="wholeTable" dxfId="6"/>
       <tableStyleElement type="headerRow" dxfId="5"/>
       <tableStyleElement type="totalRow" dxfId="4"/>
-      <tableStyleElement type="firstColumn" dxfId="3"/>
+      <tableStyleElement type="firstColumn" dxfId="2"/>
       <tableStyleElement type="lastColumn" dxfId="2"/>
-      <tableStyleElement type="firstRowStripe" dxfId="1"/>
+      <tableStyleElement type="firstRowStripe" dxfId="0"/>
       <tableStyleElement type="firstColumnStripe" dxfId="0"/>
     </tableStyle>
     <tableStyle name="PivotStylePreset2_Accent1" table="0" count="10" xr9:uid="{267968C8-6FFD-4C36-ACC1-9EA1FD1885CA}">
       <tableStyleElement type="headerRow" dxfId="16"/>
       <tableStyleElement type="totalRow" dxfId="15"/>
-      <tableStyleElement type="firstRowStripe" dxfId="14"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="13"/>
+      <tableStyleElement type="firstRowStripe" dxfId="0"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="0"/>
       <tableStyleElement type="firstSubtotalRow" dxfId="12"/>
-      <tableStyleElement type="secondSubtotalRow" dxfId="11"/>
+      <tableStyleElement type="secondSubtotalRow" dxfId="2"/>
       <tableStyleElement type="firstRowSubheading" dxfId="10"/>
       <tableStyleElement type="secondRowSubheading" dxfId="9"/>
       <tableStyleElement type="pageFieldLabels" dxfId="8"/>
@@ -1192,24 +1192,24 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="1" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="1"/>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
+    <row r="1">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2">
+    <row r="2">
+      <c r="A2" s="0">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="0" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>